<commit_message>
Solved problems from Function chapter containing game
</commit_message>
<xml_diff>
--- a/progress-sheet-of-C-How-To-Program.xlsx
+++ b/progress-sheet-of-C-How-To-Program.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CHowToProgramExcersize\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\C-How-To-Program-by-Deitel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Chapter</t>
   </si>
@@ -155,13 +155,22 @@
   </si>
   <si>
     <t>Null</t>
+  </si>
+  <si>
+    <t>Functions arguments recursion</t>
+  </si>
+  <si>
+    <t>5.10,5.12,5.09,5.26</t>
+  </si>
+  <si>
+    <t>Wrote 2 programs from solved examples: 1 Game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,15 +221,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,11 +244,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -274,12 +271,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -340,13 +336,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -755,7 +751,7 @@
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,15 +883,21 @@
       <c r="C6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E6" s="16">
         <v>3</v>
       </c>
-      <c r="F6" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="5"/>
+      <c r="F6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="15">
@@ -905,8 +907,12 @@
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="4"/>
     </row>

</xml_diff>

<commit_message>
Solved examples from function chapter
</commit_message>
<xml_diff>
--- a/progress-sheet-of-C-How-To-Program.xlsx
+++ b/progress-sheet-of-C-How-To-Program.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Chapter</t>
   </si>
@@ -151,9 +151,6 @@
     <t>completed</t>
   </si>
   <si>
-    <t>Started</t>
-  </si>
-  <si>
     <t>Null</t>
   </si>
   <si>
@@ -164,6 +161,12 @@
   </si>
   <si>
     <t>Wrote 2 programs from solved examples: 1 Game</t>
+  </si>
+  <si>
+    <t>Every aspects of Array</t>
+  </si>
+  <si>
+    <t>Pointers basics, Array and pointer, Function pointer</t>
   </si>
 </sst>
 </file>
@@ -751,7 +754,7 @@
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +808,7 @@
         <v>36</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -826,7 +829,7 @@
         <v>36</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -884,7 +887,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="16">
         <v>3</v>
@@ -893,10 +896,10 @@
         <v>36</v>
       </c>
       <c r="G6" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -906,12 +909,14 @@
       <c r="C7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="E7" s="3">
         <v>4</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="4"/>
@@ -923,9 +928,15 @@
       <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="4"/>
     </row>
@@ -938,7 +949,9 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="4"/>
     </row>

</xml_diff>

<commit_message>
2D array solved example
</commit_message>
<xml_diff>
--- a/progress-sheet-of-C-How-To-Program.xlsx
+++ b/progress-sheet-of-C-How-To-Program.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Chapter</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Pointers basics, Array and pointer, Function pointer</t>
+  </si>
+  <si>
+    <t>10 problems</t>
+  </si>
+  <si>
+    <t>6 from solved examples and 5 from exercise.</t>
   </si>
 </sst>
 </file>
@@ -753,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,8 +924,12 @@
       <c r="F7" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9">

</xml_diff>

<commit_message>
Updated status report, readme and added next problems statements
</commit_message>
<xml_diff>
--- a/progress-sheet-of-C-How-To-Program.xlsx
+++ b/progress-sheet-of-C-How-To-Program.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Chapter</t>
   </si>
@@ -169,10 +169,13 @@
     <t>Pointers basics, Array and pointer, Function pointer</t>
   </si>
   <si>
-    <t>10 problems</t>
-  </si>
-  <si>
     <t>6 from solved examples and 5 from exercise.</t>
+  </si>
+  <si>
+    <t>Around 20 problems</t>
+  </si>
+  <si>
+    <t>3 weeks</t>
   </si>
 </sst>
 </file>
@@ -759,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +773,7 @@
     <col min="4" max="4" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -918,17 +921,17 @@
       <c r="D7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="3">
-        <v>4</v>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created header file for string build in functions
</commit_message>
<xml_diff>
--- a/progress-sheet-of-C-How-To-Program.xlsx
+++ b/progress-sheet-of-C-How-To-Program.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Chapter</t>
   </si>
@@ -176,13 +176,34 @@
   </si>
   <si>
     <t>3 weeks</t>
+  </si>
+  <si>
+    <t>String build in functions</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>6 problems</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>Card game, Maze traveller are remaining.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No exercise</t>
+  </si>
+  <si>
+    <t>No exercise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +254,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +291,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -283,11 +328,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,9 +399,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -762,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,8 +1008,12 @@
       <c r="F8" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="15">
@@ -960,12 +1022,18 @@
       <c r="C9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="F9" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -977,7 +1045,9 @@
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="G10" s="19"/>
       <c r="H10" s="9"/>
     </row>
@@ -990,7 +1060,9 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="4"/>
     </row>
@@ -1003,7 +1075,9 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="G12" s="8"/>
       <c r="H12" s="4"/>
     </row>

</xml_diff>

<commit_message>
3 programs from string chapter
</commit_message>
<xml_diff>
--- a/progress-sheet-of-C-How-To-Program.xlsx
+++ b/progress-sheet-of-C-How-To-Program.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Chapter</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>No exercise</t>
+  </si>
+  <si>
+    <t>8.40 and 8.41 are remaining</t>
+  </si>
+  <si>
+    <t>Started</t>
   </si>
 </sst>
 </file>
@@ -334,7 +340,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,6 +412,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -820,22 +832,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="79.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="9">
         <v>1</v>
       </c>
@@ -879,7 +891,7 @@
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="15">
         <v>2</v>
       </c>
@@ -900,7 +912,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="9">
         <v>3</v>
       </c>
@@ -923,7 +935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="15">
         <v>4</v>
       </c>
@@ -946,7 +958,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>5</v>
       </c>
@@ -969,7 +981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="15">
         <v>6</v>
       </c>
@@ -992,7 +1004,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>7</v>
       </c>
@@ -1015,7 +1027,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="15">
         <v>8</v>
       </c>
@@ -1034,9 +1046,11 @@
       <c r="G9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>9</v>
       </c>
@@ -1051,7 +1065,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="15">
         <v>10</v>
       </c>
@@ -1066,7 +1080,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>11</v>
       </c>
@@ -1081,7 +1095,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="15">
         <v>12</v>
       </c>
@@ -1089,12 +1103,16 @@
         <v>15</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="E13" s="27">
+        <v>42840</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>56</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>13</v>
       </c>
@@ -1107,7 +1125,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="15">
         <v>14</v>
       </c>
@@ -1120,7 +1138,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>15</v>
       </c>
@@ -1133,7 +1151,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="15">
         <v>16</v>
       </c>
@@ -1146,7 +1164,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>17</v>
       </c>
@@ -1159,7 +1177,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="15">
         <v>18</v>
       </c>
@@ -1172,7 +1190,7 @@
       <c r="G19" s="18"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
         <v>19</v>
       </c>
@@ -1185,7 +1203,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="15">
         <v>20</v>
       </c>
@@ -1198,7 +1216,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="9">
         <v>21</v>
       </c>

</xml_diff>